<commit_message>
Mise à jour de l'ensemble des documents du répertoire download et doc
</commit_message>
<xml_diff>
--- a/doc/tables.xlsx
+++ b/doc/tables.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="table_subscription" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>date_demande</t>
   </si>
@@ -148,13 +146,112 @@
   </si>
   <si>
     <t>3=refusé</t>
+  </si>
+  <si>
+    <t>transaction_history</t>
+  </si>
+  <si>
+    <t>id_trans</t>
+  </si>
+  <si>
+    <t>history_date</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>id_champ</t>
+  </si>
+  <si>
+    <t>nom_champ</t>
+  </si>
+  <si>
+    <t>val_champ</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>Personnel Nexter ou conjoint</t>
+  </si>
+  <si>
+    <t>Famille Nexter (enfant)</t>
+  </si>
+  <si>
+    <t>Assistance technique, intérimaire, stagiaire, TNS ...</t>
+  </si>
+  <si>
+    <t>Retraité Nexter ou conjoint</t>
+  </si>
+  <si>
+    <t>Extérieur</t>
+  </si>
+  <si>
+    <t>field_id</t>
+  </si>
+  <si>
+    <t>field_form</t>
+  </si>
+  <si>
+    <t>val_index</t>
+  </si>
+  <si>
+    <t>dynamic_fields</t>
+  </si>
+  <si>
+    <t>field_types</t>
+  </si>
+  <si>
+    <t>field_name</t>
+  </si>
+  <si>
+    <t>adh</t>
+  </si>
+  <si>
+    <t>contrib</t>
+  </si>
+  <si>
+    <t>Codes Comptabilité</t>
+  </si>
+  <si>
+    <t>trans</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Date du certificat médical</t>
+  </si>
+  <si>
+    <t>item_id (=id_adh)</t>
+  </si>
+  <si>
+    <t>field_contents_5 (5=field_id)</t>
+  </si>
+  <si>
+    <t>field_val</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +286,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -275,6 +380,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,6 +857,159 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47627</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>130972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>678657</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107155</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5762629" y="1881189"/>
+          <a:ext cx="1690683" cy="1238249"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>23811</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>83344</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>416717</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Arc 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8441530" y="6179344"/>
+          <a:ext cx="1000125" cy="616742"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16200000"/>
+            <a:gd name="adj2" fmla="val 5399994"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>559594</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>116682</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10868026" y="5250656"/>
+          <a:ext cx="550068" cy="200026"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1047,10 +1309,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I23"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1059,9 +1322,13 @@
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1072,7 +1339,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:12">
       <c r="A2" s="12" t="s">
         <v>23</v>
       </c>
@@ -1083,7 +1350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1094,7 +1361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1110,7 +1377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1118,49 +1385,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:12">
       <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="J7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="J8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="J9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="J10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="G11" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="J11" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="J12" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="J13" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="D14" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="J14" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1171,7 +1478,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:12">
       <c r="A16" s="11" t="s">
         <v>25</v>
       </c>
@@ -1182,7 +1489,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:16">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
@@ -1193,7 +1500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:16">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -1204,7 +1511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:16">
       <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
@@ -1215,7 +1522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:16">
       <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
@@ -1229,7 +1536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
@@ -1243,7 +1550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:16">
       <c r="A22" s="9" t="s">
         <v>13</v>
       </c>
@@ -1257,41 +1564,170 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:16">
       <c r="I23" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="25" spans="1:16">
+      <c r="L25" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="L27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="L28" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="L29" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="7">
+        <v>5</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="P29" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="L30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" s="7">
+        <v>12</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="L31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N31" s="7">
+        <v>14</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="L32" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N32" s="7">
+        <v>15</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="12:16">
+      <c r="L33" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="N33" s="6">
+        <v>16</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="12:16">
+      <c r="L35" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="12:16">
+      <c r="L36" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="12:16">
+      <c r="L37" s="7">
+        <v>0</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="12:16">
+      <c r="L38" s="7">
+        <v>1</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="12:16">
+      <c r="L39" s="9">
+        <v>2</v>
+      </c>
+      <c r="M39" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="12:16">
+      <c r="L40" s="9">
+        <v>3</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="12:16">
+      <c r="L41" s="6">
+        <v>4</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>